<commit_message>
correction to text fields
Corrected translation of long vowels
</commit_message>
<xml_diff>
--- a/pref_visited.xlsx
+++ b/pref_visited.xlsx
@@ -917,7 +917,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hyōgo</t>
+          <t>Hyogo</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -947,7 +947,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kōchi</t>
+          <t>Kochi</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -1246,19 +1246,19 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Kyoto</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>京都府</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>Kyōto</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>京都府</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Kyōto</t>
-        </is>
-      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>京都市</t>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -1542,7 +1542,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ōita</t>
+          <t>Oita</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -1649,19 +1649,19 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Osaka</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>大阪府</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>Ōsaka</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>大阪府</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Ōsaka</t>
-        </is>
-      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>大阪市</t>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -1945,7 +1945,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Tōkyō</t>
+          <t>Tokyo</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
spelling correction in Tokyo
Tokyo, Hyogo, Osaka and Kyoto were corrected in the dictionary to remove the long o's.
</commit_message>
<xml_diff>
--- a/pref_visited.xlsx
+++ b/pref_visited.xlsx
@@ -877,7 +877,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>

</xml_diff>